<commit_message>
Arreglar algunos numeros faltantes
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias grupales/Matriz EDT.xlsx
+++ b/Fase 1/Evidencias grupales/Matriz EDT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Desktop\Archivos cosos git\proyecto-portal-academico-2024\Fase 1\Evidencias grupales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE9CE8D-0003-43AB-A136-B72D87EE1C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319C775E-365C-4D97-833A-0B423E05A665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="1755" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1146,9 @@
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>23</v>
+      </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
@@ -1204,7 +1206,9 @@
       <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>11</v>
+      </c>
       <c r="C21" s="6" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1273,7 @@
       </c>
       <c r="B30">
         <f>SUM(B6:B29)</f>
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1288,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -1994,13 +1998,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B34:E34"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>